<commit_message>
FileworksController and FileHelper were added.
</commit_message>
<xml_diff>
--- a/CoDA/CoDA/Files/LastTenderFile.xlsx
+++ b/CoDA/CoDA/Files/LastTenderFile.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1EFEE7D-6D57-4E31-B4A4-EAD6B8D714C8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9EDF6BC-03B0-479B-878A-272261AE0F81}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Дистрибьютор</t>
   </si>
@@ -28,7 +28,10 @@
     <t>Номер аукциона</t>
   </si>
   <si>
-    <t>Eurosevice</t>
+    <t>#1341342</t>
+  </si>
+  <si>
+    <t>Euroservice</t>
   </si>
 </sst>
 </file>
@@ -64,8 +67,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -349,7 +353,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -367,11 +371,11 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B2">
-        <v>1341342</v>
       </c>
     </row>
   </sheetData>

</xml_diff>